<commit_message>
Cambios en el presupuesto
</commit_message>
<xml_diff>
--- a/Presupuesto proyecto ADRAKODE.xlsx
+++ b/Presupuesto proyecto ADRAKODE.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\AppData\Roaming\Microsoft\Windows\Network Shortcuts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\Proyecto Marcas\adrakode.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="- AYUDA - " sheetId="4" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>DESCRIPCIÓN</t>
   </si>
@@ -114,21 +114,17 @@
   <si>
     <t xml:space="preserve">Desarrollo y Diseño inicial </t>
   </si>
-  <si>
-    <t>Servicios Adicionales y Mantenimiento</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="[$-C0A]dd\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0.00"/>
-    <numFmt numFmtId="168" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -267,7 +263,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -509,19 +505,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="dashed">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </left>
-      <right style="medium">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </right>
-      <top/>
-      <bottom style="dashed">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -610,7 +593,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -630,9 +613,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -646,9 +626,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="3" applyFill="1"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="4" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -678,7 +655,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -704,6 +680,158 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="1"/>
       <protection locked="0"/>
@@ -712,10 +840,6 @@
       <alignment horizontal="right" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -724,165 +848,13 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -2019,39 +1991,39 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4" style="29" customWidth="1"/>
-    <col min="2" max="11" width="18.44140625" style="29" customWidth="1"/>
-    <col min="12" max="16384" width="11.5546875" style="29"/>
+    <col min="1" max="1" width="4" style="26" customWidth="1"/>
+    <col min="2" max="11" width="18.44140625" style="26" customWidth="1"/>
+    <col min="12" max="16384" width="11.5546875" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="9.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:11" s="31" customFormat="1" ht="54.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-    </row>
-    <row r="3" spans="2:11" s="31" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" s="28" customFormat="1" ht="54.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+    </row>
+    <row r="3" spans="2:11" s="28" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:11" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:11" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
     </row>
     <row r="6" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
@@ -2068,7 +2040,7 @@
   <dimension ref="B1:I34"/>
   <sheetViews>
     <sheetView showGridLines="0" showZeros="0" tabSelected="1" showOutlineSymbols="0" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="H31" sqref="H31:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2085,371 +2057,364 @@
     <col min="255" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" s="13" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1" spans="2:9" s="12" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="52"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="56"/>
     </row>
     <row r="4" spans="2:9" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="57"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="37"/>
     </row>
     <row r="5" spans="2:9" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="59" t="s">
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="60">
+      <c r="H5" s="40">
         <v>321</v>
       </c>
-      <c r="I5" s="17"/>
+      <c r="I5" s="15"/>
     </row>
     <row r="6" spans="2:9" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="59" t="s">
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="64">
+      <c r="H6" s="42">
         <v>44677</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="53"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="59" t="s">
+      <c r="B7" s="33"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="66">
+      <c r="H7" s="44">
         <v>44701</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="67"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="71"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="49"/>
     </row>
     <row r="9" spans="2:9" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="74"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="64"/>
     </row>
     <row r="11" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="75" t="s">
+      <c r="B11" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="76"/>
-      <c r="D11" s="76"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="76"/>
-      <c r="H11" s="77"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="58"/>
     </row>
     <row r="12" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="75" t="s">
+      <c r="B12" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="78"/>
-      <c r="G12" s="78"/>
-      <c r="H12" s="79"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="52"/>
     </row>
     <row r="13" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="75" t="s">
+      <c r="B13" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="76"/>
-      <c r="D13" s="76"/>
-      <c r="E13" s="76"/>
-      <c r="F13" s="76"/>
-      <c r="G13" s="76"/>
-      <c r="H13" s="77"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="58"/>
     </row>
     <row r="14" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="75"/>
-      <c r="C14" s="76"/>
-      <c r="D14" s="76"/>
-      <c r="E14" s="76"/>
-      <c r="F14" s="76"/>
-      <c r="G14" s="76"/>
-      <c r="H14" s="77"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="58"/>
     </row>
     <row r="15" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="80"/>
-      <c r="C15" s="81"/>
-      <c r="D15" s="81"/>
-      <c r="E15" s="81"/>
-      <c r="F15" s="81"/>
-      <c r="G15" s="81"/>
-      <c r="H15" s="82"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="66"/>
     </row>
     <row r="16" spans="2:9" s="3" customFormat="1" ht="10.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="59"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="2:8" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="20" t="s">
+      <c r="C17" s="70"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="70"/>
+      <c r="F17" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="G17" s="20" t="s">
+      <c r="G17" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="H17" s="21" t="s">
+      <c r="H17" s="19" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="2:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="44"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="44"/>
-      <c r="F18" s="26">
+      <c r="C18" s="72"/>
+      <c r="D18" s="72"/>
+      <c r="E18" s="72"/>
+      <c r="F18" s="23">
         <v>1</v>
       </c>
-      <c r="G18" s="45">
+      <c r="G18" s="32">
         <v>600</v>
       </c>
-      <c r="H18" s="47">
+      <c r="H18" s="32">
         <f>IF(AND(F18&lt;&gt;"",G18&lt;&gt;""),F18*G18,"")</f>
         <v>600</v>
       </c>
     </row>
     <row r="19" spans="2:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="27">
+      <c r="C19" s="68"/>
+      <c r="D19" s="68"/>
+      <c r="E19" s="68"/>
+      <c r="F19" s="24">
         <v>1</v>
       </c>
-      <c r="G19" s="46">
+      <c r="G19" s="32">
         <v>900</v>
       </c>
-      <c r="H19" s="48">
+      <c r="H19" s="32">
         <f t="shared" ref="H19:H30" si="0">IF(AND(F19&lt;&gt;"",G19&lt;&gt;""),F19*G19,"")</f>
         <v>900</v>
       </c>
     </row>
     <row r="20" spans="2:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="27">
+      <c r="C20" s="68"/>
+      <c r="D20" s="68"/>
+      <c r="E20" s="68"/>
+      <c r="F20" s="24">
         <v>1</v>
       </c>
-      <c r="G20" s="46">
+      <c r="G20" s="32">
         <v>320</v>
       </c>
-      <c r="H20" s="48">
+      <c r="H20" s="32">
         <f t="shared" si="0"/>
         <v>320</v>
       </c>
     </row>
     <row r="21" spans="2:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="39" t="s">
+      <c r="B21" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="27">
+      <c r="C21" s="68"/>
+      <c r="D21" s="68"/>
+      <c r="E21" s="68"/>
+      <c r="F21" s="24">
         <v>1</v>
       </c>
-      <c r="G21" s="46">
+      <c r="G21" s="32">
         <v>120</v>
       </c>
-      <c r="H21" s="48">
+      <c r="H21" s="32">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
     </row>
     <row r="22" spans="2:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="39" t="s">
+      <c r="B22" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="27">
+      <c r="C22" s="68"/>
+      <c r="D22" s="68"/>
+      <c r="E22" s="68"/>
+      <c r="F22" s="24">
         <v>1</v>
       </c>
-      <c r="G22" s="49">
+      <c r="G22" s="32">
         <v>300</v>
       </c>
-      <c r="H22" s="48">
+      <c r="H22" s="31">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
     </row>
     <row r="23" spans="2:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="27">
+      <c r="C23" s="68"/>
+      <c r="D23" s="68"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="24">
         <v>1</v>
       </c>
-      <c r="G23" s="49">
-        <v>2000</v>
-      </c>
-      <c r="H23" s="48">
-        <f t="shared" si="0"/>
-        <v>2000</v>
+      <c r="G23" s="32">
+        <v>1100</v>
+      </c>
+      <c r="H23" s="31">
+        <v>1100</v>
       </c>
     </row>
     <row r="24" spans="2:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="27">
-        <v>1</v>
-      </c>
-      <c r="G24" s="49">
-        <v>1500</v>
-      </c>
-      <c r="H24" s="48">
-        <f t="shared" si="0"/>
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="39"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="48" t="str">
+      <c r="B24" s="67"/>
+      <c r="C24" s="68"/>
+      <c r="D24" s="68"/>
+      <c r="E24" s="68"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="31" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="39"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="49"/>
-      <c r="H26" s="48" t="str">
+    <row r="25" spans="2:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="67"/>
+      <c r="C25" s="68"/>
+      <c r="D25" s="68"/>
+      <c r="E25" s="68"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="31" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="39"/>
-      <c r="C27" s="40"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="40"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="49"/>
-      <c r="H27" s="48" t="str">
+    <row r="26" spans="2:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="67"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="68"/>
+      <c r="E26" s="68"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="31" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="39"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="40"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="49"/>
-      <c r="H28" s="10" t="str">
+    <row r="27" spans="2:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="67"/>
+      <c r="C27" s="68"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="31" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:8" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="37"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="11" t="str">
+    <row r="28" spans="2:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="67"/>
+      <c r="C28" s="68"/>
+      <c r="D28" s="68"/>
+      <c r="E28" s="68"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
+    <row r="29" spans="2:8" s="3" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="75"/>
+      <c r="C29" s="76"/>
+      <c r="D29" s="76"/>
+      <c r="E29" s="76"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
     <row r="30" spans="2:8" s="3" customFormat="1" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="16" t="str">
+      <c r="B30" s="73"/>
+      <c r="C30" s="73"/>
+      <c r="D30" s="73"/>
+      <c r="E30" s="73"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -2463,57 +2428,53 @@
       <c r="G31" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H31" s="8">
+      <c r="H31" s="77">
         <f>SUM(H18:H29)</f>
-        <v>5740</v>
+        <v>3340</v>
       </c>
     </row>
     <row r="32" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="9"/>
-      <c r="F32" s="22" t="s">
+      <c r="B32" s="8"/>
+      <c r="F32" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G32" s="23">
+      <c r="G32" s="21">
         <v>0.21</v>
       </c>
-      <c r="H32" s="14">
+      <c r="H32" s="78">
         <f>H31*G32</f>
-        <v>1205.3999999999999</v>
+        <v>701.4</v>
       </c>
     </row>
     <row r="33" spans="2:8" s="3" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="12"/>
-      <c r="C33" s="35" t="s">
+      <c r="B33" s="11"/>
+      <c r="C33" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="D33" s="35"/>
-      <c r="E33" s="35"/>
-      <c r="F33" s="35"/>
-      <c r="G33" s="35"/>
-      <c r="H33" s="24">
+      <c r="D33" s="74"/>
+      <c r="E33" s="74"/>
+      <c r="F33" s="74"/>
+      <c r="G33" s="74"/>
+      <c r="H33" s="79">
         <f>H31+H32</f>
-        <v>6945.4</v>
+        <v>4041.4</v>
       </c>
     </row>
     <row r="34" spans="2:8" s="3" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="36"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
+      <c r="B34" s="59"/>
+      <c r="C34" s="59"/>
+      <c r="D34" s="59"/>
+      <c r="E34" s="59"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="B29:E29"/>
     <mergeCell ref="B28:E28"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="B18:E18"/>
@@ -2526,10 +2487,14 @@
     <mergeCell ref="B25:E25"/>
     <mergeCell ref="B26:E26"/>
     <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C15:H15"/>
   </mergeCells>
   <pageMargins left="0.57999999999999996" right="0.2" top="0.74" bottom="1" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>

</xml_diff>